<commit_message>
ITST-16721 IPP xls2csv: wrong handling of custom format - adjust format matching, so that the custom format does correctly get replaced - adapt test
</commit_message>
<xml_diff>
--- a/tests/input_files/cell_content_test.xlsx
+++ b/tests/input_files/cell_content_test.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t>0123</t>
   </si>
@@ -51,12 +51,18 @@
   </si>
   <si>
     <t>Whitespace should not be trimmed.</t>
+  </si>
+  <si>
+    <t>Format should be interpreted correctly.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$-10409]#,##0.00;\-#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -91,6 +97,9 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -448,6 +457,14 @@
         <v>6</v>
       </c>
     </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B6" s="4">
+        <v>268.02</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>

</xml_diff>